<commit_message>
prepare 2D model for mapping model
</commit_message>
<xml_diff>
--- a/MP_ABQ_2020/Angaben_Rollmodell.xlsx
+++ b/MP_ABQ_2020/Angaben_Rollmodell.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1340760\Desktop\Rollover_ABQ_2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1340760\Desktop\abaqusrolloversimulation\MP_ABQ_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB1432B-8B68-42F9-A3B8-0487BEA79B40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CC4587-8F22-47DD-AA57-AEA83C991C87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="12036" windowHeight="7956" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="170" windowWidth="12040" windowHeight="7960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Angaben" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>Variantenname</t>
   </si>
@@ -224,10 +224,19 @@
     <t>PE</t>
   </si>
   <si>
-    <t>rollingModel-3D</t>
-  </si>
-  <si>
     <t>model_roll.py</t>
+  </si>
+  <si>
+    <t>3D-fast</t>
+  </si>
+  <si>
+    <t>2D-fast</t>
+  </si>
+  <si>
+    <t>rollingModel-2D-fast</t>
+  </si>
+  <si>
+    <t>Rolllaenge out (mm)</t>
   </si>
 </sst>
 </file>
@@ -917,22 +926,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" style="2" customWidth="1"/>
-    <col min="3" max="8" width="8.44140625" style="2" customWidth="1"/>
-    <col min="9" max="81" width="5.88671875" style="2" customWidth="1"/>
-    <col min="82" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="20.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" style="2" customWidth="1"/>
+    <col min="3" max="8" width="8.453125" style="2" customWidth="1"/>
+    <col min="9" max="81" width="5.90625" style="2" customWidth="1"/>
+    <col min="82" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="27.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -940,22 +949,22 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="D2" s="23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>45</v>
       </c>
@@ -963,15 +972,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -979,7 +988,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -987,7 +996,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -995,12 +1004,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C9" s="24">
         <v>333.26</v>
@@ -1012,7 +1021,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>2</v>
       </c>
@@ -1020,82 +1029,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B13" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C13" s="16">
         <v>-1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B14" s="21">
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B15" s="21">
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B16" s="21">
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B17" s="16">
         <v>1</v>
       </c>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B18" s="27" t="s">
         <v>1</v>
-      </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>56</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
@@ -1108,12 +1107,12 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="20">
-        <v>460</v>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
@@ -1121,15 +1120,18 @@
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="20">
-        <v>300</v>
-      </c>
-      <c r="G20" s="8"/>
+        <v>460</v>
+      </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
@@ -1137,89 +1139,104 @@
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
     </row>
-    <row r="21" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="20">
+        <v>300</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+    </row>
+    <row r="22" spans="1:17" ht="20" x14ac:dyDescent="0.4">
+      <c r="A22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F22" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="19">
-        <v>60</v>
-      </c>
-      <c r="D22" s="19">
-        <v>120</v>
-      </c>
-      <c r="E22" s="19">
+      <c r="C23" s="19">
+        <v>90</v>
+      </c>
+      <c r="D23" s="19">
+        <v>150</v>
+      </c>
+      <c r="E23" s="19">
         <v>260</v>
-      </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="19">
-        <v>25</v>
-      </c>
-      <c r="D23" s="19">
-        <v>40</v>
-      </c>
-      <c r="E23" s="19">
-        <v>80</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="19">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D24" s="19">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E24" s="19">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="19">
+        <v>14</v>
+      </c>
+      <c r="D25" s="19">
+        <v>22</v>
+      </c>
+      <c r="E25" s="19">
+        <v>35</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B26" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="19">
-        <v>3</v>
-      </c>
-      <c r="D25" s="19">
+      <c r="C26" s="19">
+        <v>2</v>
+      </c>
+      <c r="D26" s="19">
         <v>4</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E26" s="19">
         <v>10</v>
       </c>
-      <c r="F25" s="11">
-        <v>1.5</v>
-      </c>
-      <c r="G25" s="17"/>
+      <c r="F26" s="11">
+        <v>2</v>
+      </c>
+      <c r="G26" s="17"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1233,7 +1250,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
-            <xm:f>_Varianten!$A$7:$A$8</xm:f>
+            <xm:f>_Varianten!$A$7:$A$10</xm:f>
           </x14:formula1>
           <xm:sqref>B9</xm:sqref>
         </x14:dataValidation>
@@ -1241,25 +1258,25 @@
           <x14:formula1>
             <xm:f>_Varianten!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B12</xm:sqref>
+          <xm:sqref>B13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>_Varianten!$E$7:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C12</xm:sqref>
+          <xm:sqref>C13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>_Varianten!$A$12:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>B15</xm:sqref>
+          <xm:sqref>B16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>_Varianten!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B17</xm:sqref>
+          <xm:sqref>B18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
@@ -1271,7 +1288,7 @@
           <x14:formula1>
             <xm:f>_Varianten!$E$12:$E$14</xm:f>
           </x14:formula1>
-          <xm:sqref>B18</xm:sqref>
+          <xm:sqref>B19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
@@ -1290,18 +1307,18 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" customWidth="1"/>
     <col min="6" max="9" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -1312,7 +1329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1326,7 +1343,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1341,7 +1358,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1352,7 +1369,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -1360,7 +1377,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
@@ -1371,7 +1388,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1382,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1393,7 +1410,17 @@
         <v>-1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1401,7 +1428,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1410,7 +1437,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.3</v>
       </c>
@@ -1419,7 +1446,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.5</v>
       </c>
@@ -1428,34 +1455,34 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" s="14"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B16" s="14"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="14"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="14"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="14"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="14"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="14"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="14"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" s="14"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" s="14"/>
     </row>
   </sheetData>

</xml_diff>